<commit_message>
Completed functionality of constant region appending in SeqCon. with -f
</commit_message>
<xml_diff>
--- a/01_Input/Test_Table.xlsx
+++ b/01_Input/Test_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selinl/Dropbox (UMass Medical School)/dario_liisa/fran/FINAL Paper 2/ FINAL FINAL tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinseamann/Library/Mobile Documents/com~apple~CloudDocs/School/BioI-Lab/TRain/01_Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25776AA-8B87-BE49-83B3-F492B6A43698}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F46AD7-1E89-CF4F-AB63-A26536965F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="460" windowWidth="30900" windowHeight="21140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="500" windowWidth="30900" windowHeight="20500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19138,7 +19138,7 @@
   <dimension ref="A1:O711"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
-      <selection sqref="A1:M217"/>
+      <selection activeCell="E187" sqref="E187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>